<commit_message>
docs: added train_2022 components
</commit_message>
<xml_diff>
--- a/docs/TFC phase components.xlsx
+++ b/docs/TFC phase components.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kpuhger/Documents/miscCode/fiberphotopy/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyle/Library/Mobile Documents/com~apple~CloudDocs/3-Resources/code/repos/fiberphotopy/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055ECE6F-C37F-1A40-9131-57E28D492654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1234761-C87B-C244-B20F-1BD613672DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="28300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="train" sheetId="9" r:id="rId1"/>
-    <sheet name="tone" sheetId="10" r:id="rId2"/>
-    <sheet name="extinction" sheetId="11" r:id="rId3"/>
-    <sheet name="Pav_app" sheetId="17" r:id="rId4"/>
-    <sheet name="cs_response" sheetId="13" r:id="rId5"/>
-    <sheet name="shock_response" sheetId="15" r:id="rId6"/>
-    <sheet name="cs_response_2" sheetId="16" r:id="rId7"/>
+    <sheet name="train_2022" sheetId="18" r:id="rId2"/>
+    <sheet name="tone" sheetId="10" state="hidden" r:id="rId3"/>
+    <sheet name="extinction" sheetId="11" state="hidden" r:id="rId4"/>
+    <sheet name="Pav_app" sheetId="17" state="hidden" r:id="rId5"/>
+    <sheet name="cs_response" sheetId="13" state="hidden" r:id="rId6"/>
+    <sheet name="shock_response" sheetId="15" state="hidden" r:id="rId7"/>
+    <sheet name="cs_response_2" sheetId="16" state="hidden" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">extinction!$A$1:$D$82</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">tone!$A$1:$D$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">extinction!$A$1:$D$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">tone!$A$1:$D$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="233">
   <si>
     <t>baseline</t>
   </si>
@@ -1277,7 +1278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="171" zoomScaleNormal="171" zoomScalePageLayoutView="171" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="171" zoomScaleNormal="171" zoomScalePageLayoutView="171" workbookViewId="0">
       <selection activeCell="C19" sqref="C19:C20"/>
     </sheetView>
   </sheetViews>
@@ -1958,6 +1959,690 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B20D62-E86A-194F-8A17-CF8CA5FA1814}">
+  <dimension ref="A1:D42"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="171" zoomScaleNormal="171" zoomScalePageLayoutView="171" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>120</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <f>B2</f>
+        <v>120</v>
+      </c>
+      <c r="D3">
+        <f>C3+B3</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <f>D3</f>
+        <v>140</v>
+      </c>
+      <c r="D4">
+        <f>D3+B4</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <f>D4</f>
+        <v>160</v>
+      </c>
+      <c r="D5">
+        <f>D4+B5</f>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2">
+        <v>120</v>
+      </c>
+      <c r="C6">
+        <f>D5</f>
+        <v>162</v>
+      </c>
+      <c r="D6">
+        <f>D5+B6</f>
+        <v>282</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <f>D6</f>
+        <v>282</v>
+      </c>
+      <c r="D7">
+        <f>D6+B7</f>
+        <v>302</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:C42" si="0">D7</f>
+        <v>302</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ref="D8:D42" si="1">D7+B8</f>
+        <v>322</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>322</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>324</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2">
+        <v>120</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>324</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>444</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>444</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>464</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>464</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>484</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>484</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>486</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2">
+        <v>120</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>486</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>606</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>606</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>626</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="2">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>626</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>646</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>646</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>648</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="2">
+        <v>120</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>648</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>768</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="2">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>768</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>788</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="2">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>788</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>808</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>808</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>810</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="2">
+        <v>120</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>810</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>930</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="2">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>930</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>950</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="2">
+        <v>20</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>950</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>970</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>970</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>972</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="2">
+        <v>120</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>972</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="2">
+        <v>20</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>1092</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>1112</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>1132</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="2">
+        <v>120</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>1134</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="2">
+        <v>20</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>1254</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="2">
+        <v>20</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>1274</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="2">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>1294</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="2">
+        <v>120</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>1296</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="2">
+        <v>20</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>1416</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="2">
+        <v>20</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>1436</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="2">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>1456</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="1"/>
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="2">
+        <v>120</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>1458</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="1"/>
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="2">
+        <v>20</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>1578</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="2">
+        <v>20</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>1598</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="2">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>1618</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="1"/>
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="2">
+        <v>120</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>1620</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="1"/>
+        <v>1740</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D42"/>
   <sheetViews>
@@ -2642,7 +3327,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D94"/>
   <sheetViews>
@@ -4003,7 +4688,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82A8FD94-CD39-6740-9FD5-CD8226346013}">
   <dimension ref="A1:E95"/>
   <sheetViews>
@@ -5545,7 +6230,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D82"/>
   <sheetViews>
@@ -6869,7 +7554,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D82"/>
   <sheetViews>
@@ -7699,12 +8384,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="171" zoomScaleNormal="171" zoomScalePageLayoutView="171" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>